<commit_message>
Additional simulation files and small edits
</commit_message>
<xml_diff>
--- a/AlternativeVersions/2_withAsymmetricSteadyState/steady_state_numbers.xlsx
+++ b/AlternativeVersions/2_withAsymmetricSteadyState/steady_state_numbers.xlsx
@@ -28,8 +28,8 @@
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="34" r:id="rId9"/>
-    <pivotCache cacheId="35" r:id="rId10"/>
+    <pivotCache cacheId="38" r:id="rId9"/>
+    <pivotCache cacheId="39" r:id="rId10"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -5086,7 +5086,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C137F86C-18A2-4ADE-B136-CA67840DF6E0}" type="CELLRANGE">
+                    <a:fld id="{32A5F332-9A03-4B02-9270-F210EA04D54D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5120,7 +5120,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F60E8990-5821-4177-B7B2-55BD3614457B}" type="CELLRANGE">
+                    <a:fld id="{0F5BC3DC-782E-40D1-85D2-13147B420E76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5154,7 +5154,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA6D0784-C691-48B1-A92E-4F4FD7653893}" type="CELLRANGE">
+                    <a:fld id="{0674882B-2DAA-4374-BD57-348FAC4360F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5188,7 +5188,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{330F0E7D-33AC-4698-BC49-DFF38B21F6ED}" type="CELLRANGE">
+                    <a:fld id="{4FB72833-807F-4789-AFF1-4C9E5F8171AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5222,7 +5222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6284126-345A-484F-9B92-B2254E75213A}" type="CELLRANGE">
+                    <a:fld id="{0EB26487-459B-45D5-AA6E-80EDE739522A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5256,7 +5256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CF02224-2173-42C9-819C-48D19C7B73CB}" type="CELLRANGE">
+                    <a:fld id="{F9C521EE-4AA8-42F5-AF41-08D66CE7CFD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5290,7 +5290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9056A9D6-A48F-48B7-85FA-3EF1EE194574}" type="CELLRANGE">
+                    <a:fld id="{1A320066-D6C1-4C2E-9564-88FD2F898E3E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5324,7 +5324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3E01666-DD0E-4082-9BF4-AD0B49EBB83C}" type="CELLRANGE">
+                    <a:fld id="{3B276013-0358-4CD7-9849-0346C7AACBDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6409,7 +6409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{327E7E9A-1504-4971-A1CB-6E0C844E97A7}" type="CELLRANGE">
+                    <a:fld id="{2A93FDC7-043B-4088-80A0-8F13192BDEF9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6443,7 +6443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1111D03A-2222-49B4-8655-9437E9FE63B8}" type="CELLRANGE">
+                    <a:fld id="{CE0ED7B1-6991-4641-83D0-0BB551B1A052}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6477,7 +6477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92DFBFD7-E7F9-4803-80D1-1184F4DFB990}" type="CELLRANGE">
+                    <a:fld id="{BB835DD1-D071-4008-A375-D16721D52CED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6511,7 +6511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{681E26BE-C87C-4FAE-9FC5-37E74E5F0B18}" type="CELLRANGE">
+                    <a:fld id="{422CB622-DB15-4C08-BAB1-7019A7AF6EC8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6545,7 +6545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C4C40BD-C1B8-4B40-AEB3-E33D11F2FBAA}" type="CELLRANGE">
+                    <a:fld id="{72F7D986-9F48-4566-8BB7-E77564F25920}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6579,7 +6579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECD0F133-FC62-48D2-9F80-C248A48797AA}" type="CELLRANGE">
+                    <a:fld id="{AF59DB40-DC6F-47B2-B88F-FBE8BBF43FFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6613,7 +6613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E5461C6-34A3-4C46-8641-00843E96415C}" type="CELLRANGE">
+                    <a:fld id="{41913492-DC2E-482F-A795-33E4A213E63C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6647,7 +6647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAA041B3-B55D-4811-BBC1-259644CD4F96}" type="CELLRANGE">
+                    <a:fld id="{A9C0E20D-5A31-40C8-9685-209152F8791D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7672,7 +7672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D55C415-6328-42CB-8C70-E21E478E7B16}" type="CELLRANGE">
+                    <a:fld id="{C0E368A0-D295-4E72-8800-5128F88E2619}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7706,7 +7706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14E8977B-4FC9-445A-A16F-BF41552F603E}" type="CELLRANGE">
+                    <a:fld id="{D0C53051-5190-4F20-B920-CC2240499D46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7740,7 +7740,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90C14A27-DBE4-45F3-BEAE-4980833EFA21}" type="CELLRANGE">
+                    <a:fld id="{7EDFAE47-77E9-4AB5-82CA-5B58FDDB140A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7774,7 +7774,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82F932CF-4738-475B-86D6-D7BD8A61CDB1}" type="CELLRANGE">
+                    <a:fld id="{5FA436BC-B945-4FF2-9325-C9215AF8396E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7808,7 +7808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{688B686B-4445-44FF-A8FF-AADB507E3C4E}" type="CELLRANGE">
+                    <a:fld id="{01E44E54-E280-45C2-AFB3-445D41087F3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7842,7 +7842,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{244F3688-EA38-493E-9535-83B3C3407167}" type="CELLRANGE">
+                    <a:fld id="{CC397E9C-0B7C-406D-8438-C4E98FEDBF39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7876,7 +7876,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{246A7F94-F743-4FED-9B4D-73A0724A79CF}" type="CELLRANGE">
+                    <a:fld id="{28845C9D-1809-4605-BBFE-81088A1C18DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7910,7 +7910,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77ABE708-2B5B-4ECA-8A79-E661D9732B98}" type="CELLRANGE">
+                    <a:fld id="{570A2C66-E81F-4F4E-B52A-2A1EE538D38D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8932,7 +8932,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0940F0B6-2626-43DA-9AFF-B8A0E4149ACA}" type="CELLRANGE">
+                    <a:fld id="{D3C228C9-5068-45AB-8682-01B513515587}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8966,7 +8966,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A338786F-5722-4ACF-9AE7-E4B60F72421B}" type="CELLRANGE">
+                    <a:fld id="{A47B8040-DBFF-4346-8DAC-7163B345B5BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9000,7 +9000,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C737D9C3-930F-453B-8B0E-CAA7D6D72CBB}" type="CELLRANGE">
+                    <a:fld id="{D050F1E6-592D-4DBE-B48D-76CAF6662226}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9034,7 +9034,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03367F25-5C97-4124-8676-82FA66940898}" type="CELLRANGE">
+                    <a:fld id="{41F88102-43B5-4D15-8CBF-F7E597661AD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9068,7 +9068,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EB43891-D419-42BF-A5DB-FD674B501851}" type="CELLRANGE">
+                    <a:fld id="{C6826181-60CA-4422-94E4-9F06BC026868}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9102,7 +9102,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9F23978-D65E-4561-B21D-E9CE8B053539}" type="CELLRANGE">
+                    <a:fld id="{0F4FECA9-DE37-4B20-A301-77EC51E60E3A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9136,7 +9136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E889B86A-B8C4-4D5F-A3B4-9FA454558D6C}" type="CELLRANGE">
+                    <a:fld id="{77419FEA-1126-4674-9E43-27809C97B467}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9170,7 +9170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{141B83B5-1E23-47AA-94E9-D18D2358AC39}" type="CELLRANGE">
+                    <a:fld id="{9EE55965-636C-45BC-9297-302DA458330E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -41573,7 +41573,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:I11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisPage" subtotalTop="0" showAll="0">
@@ -41750,7 +41750,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:I11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -41927,7 +41927,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:I6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisPage" subtotalTop="0" showAll="0">
@@ -42079,7 +42079,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -42576,11 +42576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P230"/>
+  <dimension ref="A1:P240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:N230"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:N240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53575,6 +53575,446 @@
         <v>11.516409439731079</v>
       </c>
       <c r="N230">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>0.7994</v>
+      </c>
+      <c r="B231">
+        <v>1.7</v>
+      </c>
+      <c r="C231">
+        <v>0.05</v>
+      </c>
+      <c r="D231">
+        <v>4</v>
+      </c>
+      <c r="E231">
+        <v>2</v>
+      </c>
+      <c r="F231">
+        <v>8</v>
+      </c>
+      <c r="G231">
+        <v>0.2</v>
+      </c>
+      <c r="H231">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I231">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J231">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K231">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L231">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M231">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N231">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>0.7994</v>
+      </c>
+      <c r="B232">
+        <v>1.7</v>
+      </c>
+      <c r="C232">
+        <v>0.05</v>
+      </c>
+      <c r="D232">
+        <v>4</v>
+      </c>
+      <c r="E232">
+        <v>2</v>
+      </c>
+      <c r="F232">
+        <v>8</v>
+      </c>
+      <c r="G232">
+        <v>0.2</v>
+      </c>
+      <c r="H232">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I232">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J232">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K232">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L232">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M232">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N232">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>0.7994</v>
+      </c>
+      <c r="B233">
+        <v>1.7</v>
+      </c>
+      <c r="C233">
+        <v>0.05</v>
+      </c>
+      <c r="D233">
+        <v>4</v>
+      </c>
+      <c r="E233">
+        <v>2</v>
+      </c>
+      <c r="F233">
+        <v>8</v>
+      </c>
+      <c r="G233">
+        <v>0.2</v>
+      </c>
+      <c r="H233">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I233">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J233">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K233">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L233">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M233">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N233">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>0.7994</v>
+      </c>
+      <c r="B234">
+        <v>1.7</v>
+      </c>
+      <c r="C234">
+        <v>0.05</v>
+      </c>
+      <c r="D234">
+        <v>4</v>
+      </c>
+      <c r="E234">
+        <v>2</v>
+      </c>
+      <c r="F234">
+        <v>8</v>
+      </c>
+      <c r="G234">
+        <v>0.2</v>
+      </c>
+      <c r="H234">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I234">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J234">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K234">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L234">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M234">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N234">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>0.7994</v>
+      </c>
+      <c r="B235">
+        <v>1.7</v>
+      </c>
+      <c r="C235">
+        <v>0.05</v>
+      </c>
+      <c r="D235">
+        <v>4</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+      <c r="F235">
+        <v>8</v>
+      </c>
+      <c r="G235">
+        <v>0.2</v>
+      </c>
+      <c r="H235">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I235">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J235">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K235">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L235">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M235">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N235">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>0.7994</v>
+      </c>
+      <c r="B236">
+        <v>1.7</v>
+      </c>
+      <c r="C236">
+        <v>0.05</v>
+      </c>
+      <c r="D236">
+        <v>4</v>
+      </c>
+      <c r="E236">
+        <v>2</v>
+      </c>
+      <c r="F236">
+        <v>8</v>
+      </c>
+      <c r="G236">
+        <v>0.2</v>
+      </c>
+      <c r="H236">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I236">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J236">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K236">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L236">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M236">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N236">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>0.7994</v>
+      </c>
+      <c r="B237">
+        <v>1.7</v>
+      </c>
+      <c r="C237">
+        <v>0.05</v>
+      </c>
+      <c r="D237">
+        <v>4</v>
+      </c>
+      <c r="E237">
+        <v>2</v>
+      </c>
+      <c r="F237">
+        <v>8</v>
+      </c>
+      <c r="G237">
+        <v>0.2</v>
+      </c>
+      <c r="H237">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I237">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J237">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K237">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L237">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M237">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N237">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>0.7994</v>
+      </c>
+      <c r="B238">
+        <v>1.7</v>
+      </c>
+      <c r="C238">
+        <v>0.05</v>
+      </c>
+      <c r="D238">
+        <v>4</v>
+      </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
+      <c r="F238">
+        <v>8</v>
+      </c>
+      <c r="G238">
+        <v>0.2</v>
+      </c>
+      <c r="H238">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I238">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J238">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K238">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L238">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M238">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N238">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>0.7994</v>
+      </c>
+      <c r="B239">
+        <v>1.7</v>
+      </c>
+      <c r="C239">
+        <v>0.05</v>
+      </c>
+      <c r="D239">
+        <v>4</v>
+      </c>
+      <c r="E239">
+        <v>4</v>
+      </c>
+      <c r="F239">
+        <v>8</v>
+      </c>
+      <c r="G239">
+        <v>0.2</v>
+      </c>
+      <c r="H239">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I239">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J239">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K239">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L239">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M239">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N239">
+        <v>1.1156885869537867</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>0.7994</v>
+      </c>
+      <c r="B240">
+        <v>1.7</v>
+      </c>
+      <c r="C240">
+        <v>0.05</v>
+      </c>
+      <c r="D240">
+        <v>4</v>
+      </c>
+      <c r="E240">
+        <v>4</v>
+      </c>
+      <c r="F240">
+        <v>8</v>
+      </c>
+      <c r="G240">
+        <v>0.2</v>
+      </c>
+      <c r="H240">
+        <v>12.717330992320706</v>
+      </c>
+      <c r="I240">
+        <v>21.002061227290888</v>
+      </c>
+      <c r="J240">
+        <v>1.1003425448650146</v>
+      </c>
+      <c r="K240">
+        <v>0.92394242418103889</v>
+      </c>
+      <c r="L240">
+        <v>1.1277996692059085</v>
+      </c>
+      <c r="M240">
+        <v>11.516409439731079</v>
+      </c>
+      <c r="N240">
         <v>1.1156885869537867</v>
       </c>
     </row>

</xml_diff>